<commit_message>
added http update server and arduino OTA lib, changed pinout
</commit_message>
<xml_diff>
--- a/JKW_MQTT_PWM_PIR_TEMP/documentation/pinout.xlsx
+++ b/JKW_MQTT_PWM_PIR_TEMP/documentation/pinout.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="72">
   <si>
     <t>antenna</t>
   </si>
@@ -399,18 +399,12 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -422,14 +416,8 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="3" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -446,6 +434,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="60% - Accent4" xfId="4" builtinId="44"/>
@@ -762,7 +759,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -777,25 +774,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="19" t="s">
         <v>69</v>
       </c>
     </row>
@@ -809,13 +806,13 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="18" t="s">
+      <c r="E2" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -829,13 +826,13 @@
       <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="18" t="s">
+      <c r="E3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -849,13 +846,13 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="18" t="s">
+      <c r="E4" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -869,13 +866,13 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="18" t="s">
+      <c r="E5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -889,13 +886,13 @@
       <c r="C6" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="18" t="s">
+      <c r="E6" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -909,13 +906,13 @@
       <c r="C7" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="16" t="s">
         <v>58</v>
       </c>
     </row>
@@ -932,13 +929,13 @@
       <c r="D8" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="18" t="s">
+      <c r="E8" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -955,24 +952,24 @@
       <c r="D9" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="18" t="s">
+      <c r="E9" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -984,13 +981,13 @@
       <c r="C11" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="17" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1004,13 +1001,13 @@
       <c r="C12" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="7" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1024,13 +1021,13 @@
       <c r="C13" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="13" t="s">
+      <c r="E13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1047,13 +1044,13 @@
       <c r="D14" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="2" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1067,16 +1064,16 @@
       <c r="C15" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="12" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1090,13 +1087,13 @@
       <c r="C16" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="16" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1110,11 +1107,11 @@
       <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="8" t="s">
+      <c r="F17" s="22"/>
+      <c r="G17" s="6" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1131,19 +1128,21 @@
       <c r="E18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="20" t="s">
+      <c r="F18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="16" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="12"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
@@ -1155,13 +1154,13 @@
       <c r="C20" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G20" s="18" t="s">
+      <c r="E20" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1178,13 +1177,13 @@
       <c r="D21" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G21" s="18" t="s">
+      <c r="E21" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G21" s="14" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1201,13 +1200,13 @@
       <c r="D22" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G22" s="18" t="s">
+      <c r="E22" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" s="14" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1224,13 +1223,13 @@
       <c r="D23" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G23" s="18" t="s">
+      <c r="E23" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" s="14" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1247,13 +1246,13 @@
       <c r="D24" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G24" s="18" t="s">
+      <c r="E24" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="14" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1270,13 +1269,13 @@
       <c r="D25" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G25" s="18" t="s">
+      <c r="E25" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G25" s="14" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1293,13 +1292,13 @@
       <c r="D26" t="s">
         <v>50</v>
       </c>
-      <c r="E26" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G26" s="18" t="s">
+      <c r="E26" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="14" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1313,24 +1312,24 @@
       <c r="C27" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="G27" s="16" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="19"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="12"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="9"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
@@ -1345,13 +1344,13 @@
       <c r="D29" t="s">
         <v>52</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="G29" s="5" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1368,13 +1367,13 @@
       <c r="D30" t="s">
         <v>52</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="G30" s="5" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1388,13 +1387,13 @@
       <c r="C31" t="s">
         <v>22</v>
       </c>
-      <c r="E31" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F31" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G31" s="18" t="s">
+      <c r="E31" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G31" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1408,13 +1407,13 @@
       <c r="C32" t="s">
         <v>23</v>
       </c>
-      <c r="E32" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F32" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G32" s="18" t="s">
+      <c r="E32" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G32" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1428,13 +1427,13 @@
       <c r="C33" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F33" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G33" s="18" t="s">
+      <c r="E33" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G33" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1448,13 +1447,13 @@
       <c r="C34" t="s">
         <v>7</v>
       </c>
-      <c r="E34" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F34" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G34" s="18" t="s">
+      <c r="E34" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G34" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1468,13 +1467,13 @@
       <c r="C35" t="s">
         <v>24</v>
       </c>
-      <c r="E35" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F35" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" s="18" t="s">
+      <c r="E35" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G35" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1491,24 +1490,24 @@
       <c r="D36" t="s">
         <v>53</v>
       </c>
-      <c r="E36" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F36" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G36" s="18" t="s">
+      <c r="E36" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G36" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="19"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="12"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="9"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
@@ -1517,28 +1516,27 @@
       <c r="C38" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="19"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="12"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
+    <mergeCell ref="E10:F10"/>
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
     <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>